<commit_message>
Implemented adjust and rewrote the dates for deposit helper
</commit_message>
<xml_diff>
--- a/functions (version 1).xlsx
+++ b/functions (version 1).xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiarf\Documents\GitHub\bootstrapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DD97339-B5C5-41F4-A4CA-263CF54BCAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F88744-4745-42B5-B657-845D3A1E1292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="times" sheetId="1" r:id="rId1"/>
     <sheet name="solver" sheetId="4" r:id="rId2"/>
     <sheet name="LinearInterpolation.hpp" sheetId="6" r:id="rId3"/>
     <sheet name="forecastfixing test" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="FixingDays" sheetId="3" r:id="rId6"/>
-    <sheet name="FixingDays21" sheetId="5" r:id="rId7"/>
+    <sheet name="FRARATEHELPER" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="FixingDays" sheetId="3" r:id="rId8"/>
+    <sheet name="FixingDays21" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>d1</t>
   </si>
@@ -130,6 +131,42 @@
   </si>
   <si>
     <t>printing</t>
+  </si>
+  <si>
+    <t>ImpledQuote</t>
+  </si>
+  <si>
+    <t>useIndexedCoupon_ is set to True</t>
+  </si>
+  <si>
+    <t>9/18/2013</t>
+  </si>
+  <si>
+    <t>reference_date</t>
+  </si>
+  <si>
+    <t>earliest_date</t>
+  </si>
+  <si>
+    <t>fixing_date</t>
+  </si>
+  <si>
+    <t>maturity_date</t>
+  </si>
+  <si>
+    <t>pillar_date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Deposit1</t>
+  </si>
+  <si>
+    <t>Deposit2</t>
   </si>
 </sst>
 </file>
@@ -139,7 +176,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.000000000000_-;\-* #,##0.000000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,7 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -979,21 +1016,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>210430</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>162081</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>48653</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38371</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6059B444-7105-198F-0F2D-1F63ED861CB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E51CE50-D6B7-91A6-49FE-50AB54F44D12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1009,8 +1046,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="762000"/>
-          <a:ext cx="6306430" cy="1114581"/>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="7363853" cy="1943371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>325086</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89169E03-10F6-3F9C-E1FF-2F95BAA92B63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2286000"/>
+          <a:ext cx="8859486" cy="3372321"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>591856</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>124564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9BAE224-54FF-9476-425D-D8F588199C10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11353800" y="542925"/>
+          <a:ext cx="9354856" cy="5296639"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1028,6 +1153,55 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>210430</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>162081</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6059B444-7105-198F-0F2D-1F63ED861CB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="762000"/>
+          <a:ext cx="6306430" cy="1114581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1159,7 +1333,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1637,18 +1811,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F8CA2-E401-43A6-95C3-FB9801E4079C}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1656,7 +1834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>44929</v>
       </c>
@@ -1664,7 +1842,7 @@
         <v>44930</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44929</v>
       </c>
@@ -1675,15 +1853,142 @@
         <v>44929</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>44929</v>
       </c>
+      <c r="D5" s="1">
+        <f>C5+94</f>
+        <v>45023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44925</v>
+      </c>
+      <c r="C8">
+        <v>44925</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44925</v>
+      </c>
+      <c r="F8">
+        <v>44925</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44929</v>
+      </c>
+      <c r="C9">
+        <v>44929</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44929</v>
+      </c>
+      <c r="F9">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44925</v>
+      </c>
+      <c r="C10">
+        <v>44925</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44925</v>
+      </c>
+      <c r="F10">
+        <v>44925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44930</v>
+      </c>
+      <c r="C11">
+        <v>44930</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45019</v>
+      </c>
+      <c r="F11">
+        <v>45019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44930</v>
+      </c>
+      <c r="C12">
+        <v>44930</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45019</v>
+      </c>
+      <c r="F12">
+        <v>45019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1819,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9121186-4CCD-40A7-982B-7FC227AF05BA}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,6 +2304,106 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64CCBA5-7B10-4EB2-8AB4-056560FADA49}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" s="1" t="e">
+        <f>DATE(YEAR(S1), MONTH(S1) + 3, 1 + MOD(4 - WEEKDAY(DATE(YEAR(S1), MONTH(S1) + 3, 1)), 7) + 14)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B4B971-C409-45D5-89E4-3CECF6C0C255}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>DATE(YEAR(A1), MONTH(A1) + 3, 1 + MOD(4 - WEEKDAY(DATE(YEAR(A1), MONTH(A1) + 3, 1)), 7) + 14)</f>
+        <v>45035</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A8" si="0">DATE(YEAR(A2), MONTH(A2) + 3, 1 + MOD(4 - WEEKDAY(DATE(YEAR(A2), MONTH(A2) + 3, 1)), 7) + 14)</f>
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>45217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>45399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>45490</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>45581</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD78AF61-420F-400B-9D02-C5DDBB30AD29}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -2034,7 +2439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AF91E-0D3B-411F-A339-01B8AFAB9B6E}">
   <dimension ref="A33"/>
   <sheetViews>
@@ -2055,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796BF369-BDB9-4727-9C6A-D1AB0BD2A96D}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Found issue with maturity date for FRA
</commit_message>
<xml_diff>
--- a/functions (version 1).xlsx
+++ b/functions (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiarf\Documents\GitHub\bootstrapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DEC34B-B108-4D80-99E6-D840FF8DC2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F84CAED-0686-467C-ACE9-4802DC5BCB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
   </bookViews>
@@ -1817,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F8CA2-E401-43A6-95C3-FB9801E4079C}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="G12" sqref="G12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,9 +1833,10 @@
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>44929</v>
       </c>
@@ -1851,7 +1852,7 @@
         <v>44930</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44929</v>
       </c>
@@ -1862,12 +1863,12 @@
         <v>44929</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>44929</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>45023</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1928,7 +1929,7 @@
         <v>44925</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1956,8 +1957,14 @@
       <c r="I9" s="1">
         <v>44929</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>45098</v>
+      </c>
+      <c r="L9" s="1">
+        <v>45098</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1985,8 +1992,14 @@
       <c r="I10" s="1">
         <v>45000</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>45092</v>
+      </c>
+      <c r="L10" s="1">
+        <v>45092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2014,8 +2027,11 @@
       <c r="I11" s="1">
         <v>44998</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -2038,13 +2054,13 @@
         <v>35</v>
       </c>
       <c r="H12">
-        <v>45092</v>
+        <v>45098</v>
       </c>
       <c r="I12" s="1">
-        <v>45092</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="G13" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Setting up fixed rate coupons
</commit_message>
<xml_diff>
--- a/functions (version 1).xlsx
+++ b/functions (version 1).xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiarf\Documents\GitHub\bootstrapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F84CAED-0686-467C-ACE9-4802DC5BCB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E664ADE-B5BA-409F-99CD-E65A76046BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="times" sheetId="1" r:id="rId1"/>
-    <sheet name="solver" sheetId="4" r:id="rId2"/>
-    <sheet name="LinearInterpolation.hpp" sheetId="6" r:id="rId3"/>
-    <sheet name="forecastfixing test" sheetId="7" r:id="rId4"/>
-    <sheet name="FRARATEHELPER" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
-    <sheet name="FixingDays" sheetId="3" r:id="rId8"/>
-    <sheet name="FixingDays21" sheetId="5" r:id="rId9"/>
+    <sheet name="swap_times" sheetId="10" r:id="rId2"/>
+    <sheet name="solver" sheetId="4" r:id="rId3"/>
+    <sheet name="LinearInterpolation.hpp" sheetId="6" r:id="rId4"/>
+    <sheet name="forecastfixing test" sheetId="7" r:id="rId5"/>
+    <sheet name="FRARATEHELPER" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
+    <sheet name="FixingDays" sheetId="3" r:id="rId9"/>
+    <sheet name="FixingDays21" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>d1</t>
   </si>
@@ -173,6 +174,9 @@
   </si>
   <si>
     <t>spot_date</t>
+  </si>
+  <si>
+    <t>schedule</t>
   </si>
 </sst>
 </file>
@@ -200,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +223,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -233,13 +243,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1819,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F8CA2-E401-43A6-95C3-FB9801E4079C}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12:I13"/>
     </sheetView>
   </sheetViews>
@@ -2077,7 +2088,69 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796BF369-BDB9-4727-9C6A-D1AB0BD2A96D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="X79" sqref="X79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBA1329-2698-47D3-94BF-E5D893A31A2A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>44929</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>45110</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>45294</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E38CA1-BBFC-4859-A4B2-B5A2F673F30B}">
   <dimension ref="A50:Z66"/>
   <sheetViews>
@@ -2146,7 +2219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84A4595-A806-403B-96F7-B5AA7B799DF5}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -2202,7 +2275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9121186-4CCD-40A7-982B-7FC227AF05BA}">
   <dimension ref="A1:G20"/>
   <sheetViews>
@@ -2385,7 +2458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64CCBA5-7B10-4EB2-8AB4-056560FADA49}">
   <dimension ref="A1:S4"/>
   <sheetViews>
@@ -2420,7 +2493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B4B971-C409-45D5-89E4-3CECF6C0C255}">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -2485,7 +2558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD78AF61-420F-400B-9D02-C5DDBB30AD29}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -2521,7 +2594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AF91E-0D3B-411F-A339-01B8AFAB9B6E}">
   <dimension ref="A33"/>
   <sheetViews>
@@ -2540,19 +2613,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796BF369-BDB9-4727-9C6A-D1AB0BD2A96D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="X79" sqref="X79"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>